<commit_message>
Starting on energy calcs
</commit_message>
<xml_diff>
--- a/custom sim/FEB_SN3_30kW.xlsx
+++ b/custom sim/FEB_SN3_30kW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Westo\OneDrive\Documents\School\FEB\Git\OpenLap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EJDRO\OneDrive\Documents\GitHub\FEBSim\custom sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706CE374-92A3-49F4-8477-0C6513415F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82626EC8-3FA0-4099-A65C-6F5D8D68D854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -771,6 +771,1203 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Torque Curve'!$A$2:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>7.0159375299999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.662052770000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>157.92182149999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>265.18159020000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>372.44135899999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>479.70112769999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>586.96089640000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>694.22066510000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>801.78514910000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>908.74020259999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1015.999971</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1123.25974</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1230.519509</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1331.075542</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1438.335311</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1545.5950789999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1652.8548479999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1760.114617</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1867.374386</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1974.6341540000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2081.8939230000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2189.1536919999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2296.4134610000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2403.3685139999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2510.9329980000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2612.6063199999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2720.7599209999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2826.0085690000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2933.268337</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3040.5281060000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3140.0879020000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3210.749726</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3309.794817</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3415.9372969999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3523.1970649999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3630.4568340000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3737.7166029999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3844.9763720000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3945.5324049999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4053.7063189999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4160.0519420000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4267.3117110000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4374.5714799999996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4480.9171029999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4589.0910169999997</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4694.3396650000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4801.4775479999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4907.5184550000004</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5014.7782239999997</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5122.0379929999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5227.957015</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5326.5019270000003</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5433.4569810000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Torque Curve'!$B$2:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>230.2535546</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>230.3330272</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230.21973080000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>220.41915</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>205.12270710000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>191.8115478</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180.12272809999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>169.7766924</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>160.5546253</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>152.28280520000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>144.8215572</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>138.05730199999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>131.913456</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>126.2624876</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>121.3488019</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>116.5250356</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>112.1853097</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>108.0830699</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>104.27025690000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100.9642585</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>98.742248290000006</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>95.787401990000006</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>92.811026400000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>89.985499189999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>87.326929129999996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>84.820942919999993</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>82.454771100000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>80.353324749999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>78.209081190000006</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>76.209780809999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>74.294232089999994</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>72.472617740000004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>70.752624819999994</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>69.084846099999993</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>67.535940999999994</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>66.028976180000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>64.602232180000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>63.22047207</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>61.896582389999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>60.642550370000002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>59.520610519999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>58.348975199999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C735-440B-98EC-7DC20B1DE613}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="787399071"/>
+        <c:axId val="640127855"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="787399071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="640127855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="640127855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="787399071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>407670</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BF2E6BA-8F7B-0CA4-309B-5AE41917F3B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1049,20 +2246,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="22" t="s">
         <v>45</v>
       </c>
@@ -1079,7 +2276,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
@@ -1096,7 +2293,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="35"/>
       <c r="B3" s="11" t="s">
         <v>2</v>
@@ -1109,7 +2306,7 @@
       </c>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="34" t="s">
         <v>12</v>
       </c>
@@ -1126,7 +2323,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="35"/>
       <c r="B5" s="11" t="s">
         <v>4</v>
@@ -1139,7 +2336,7 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
@@ -1154,7 +2351,7 @@
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
@@ -1171,7 +2368,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="34" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +2385,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="36"/>
       <c r="B9" s="1" t="s">
         <v>74</v>
@@ -1203,7 +2400,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="36"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -1216,7 +2413,7 @@
       </c>
       <c r="E10" s="20"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="36"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -1229,7 +2426,7 @@
       </c>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="36"/>
       <c r="B12" s="1" t="s">
         <v>72</v>
@@ -1242,7 +2439,7 @@
       </c>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="36"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
@@ -1255,7 +2452,7 @@
       </c>
       <c r="E13" s="20"/>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="35"/>
       <c r="B14" s="11" t="s">
         <v>23</v>
@@ -1270,7 +2467,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="34" t="s">
         <v>20</v>
       </c>
@@ -1287,7 +2484,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="36"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
@@ -1302,7 +2499,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="36"/>
       <c r="B17" s="1" t="s">
         <v>78</v>
@@ -1317,7 +2514,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="36"/>
       <c r="B18" s="1" t="s">
         <v>26</v>
@@ -1332,7 +2529,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="36"/>
       <c r="B19" s="1" t="s">
         <v>27</v>
@@ -1347,7 +2544,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="36"/>
       <c r="B20" s="1" t="s">
         <v>28</v>
@@ -1362,7 +2559,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="35"/>
       <c r="B21" s="11" t="s">
         <v>29</v>
@@ -1377,7 +2574,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A22" s="34" t="s">
         <v>30</v>
       </c>
@@ -1392,7 +2589,7 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="36"/>
       <c r="B23" s="1" t="s">
         <v>31</v>
@@ -1407,7 +2604,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="36"/>
       <c r="B24" s="1" t="s">
         <v>36</v>
@@ -1422,13 +2619,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="36"/>
       <c r="B25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="3">
-        <v>1.4</v>
+        <v>1.64</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>38</v>
@@ -1437,7 +2634,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="36"/>
       <c r="B26" s="1" t="s">
         <v>33</v>
@@ -1452,7 +2649,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="36"/>
       <c r="B27" s="1" t="s">
         <v>34</v>
@@ -1467,13 +2664,13 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="36"/>
       <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="3">
-        <v>1.4</v>
+        <v>1.64</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>38</v>
@@ -1482,7 +2679,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="36"/>
       <c r="B29" s="1" t="s">
         <v>40</v>
@@ -1497,7 +2694,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="36"/>
       <c r="B30" s="1" t="s">
         <v>41</v>
@@ -1512,7 +2709,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="36"/>
       <c r="B31" s="1" t="s">
         <v>42</v>
@@ -1527,7 +2724,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="35"/>
       <c r="B32" s="11" t="s">
         <v>43</v>
@@ -1542,7 +2739,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="34" t="s">
         <v>50</v>
       </c>
@@ -1557,7 +2754,7 @@
       </c>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="36"/>
       <c r="B34" s="1" t="s">
         <v>52</v>
@@ -1572,7 +2769,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="35"/>
       <c r="B35" s="11" t="s">
         <v>53</v>
@@ -1587,7 +2784,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="31" t="s">
         <v>55</v>
       </c>
@@ -1602,7 +2799,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="32"/>
       <c r="B37" s="4" t="s">
         <v>79</v>
@@ -1617,7 +2814,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="32"/>
       <c r="B38" s="4" t="s">
         <v>75</v>
@@ -1632,7 +2829,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="32"/>
       <c r="B39" s="4" t="s">
         <v>76</v>
@@ -1647,7 +2844,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="32"/>
       <c r="B40" s="4" t="s">
         <v>77</v>
@@ -1662,7 +2859,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="32"/>
       <c r="B41" s="1" t="s">
         <v>60</v>
@@ -1677,7 +2874,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="32"/>
       <c r="B42" s="1" t="s">
         <v>61</v>
@@ -1690,7 +2887,7 @@
       </c>
       <c r="E42" s="20"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="32"/>
       <c r="B43" s="26" t="s">
         <v>62</v>
@@ -1703,7 +2900,7 @@
       </c>
       <c r="E43" s="20"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="32"/>
       <c r="B44" s="26" t="s">
         <v>63</v>
@@ -1714,7 +2911,7 @@
       </c>
       <c r="E44" s="20"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="32"/>
       <c r="B45" s="26" t="s">
         <v>64</v>
@@ -1725,7 +2922,7 @@
       </c>
       <c r="E45" s="20"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="32"/>
       <c r="B46" s="26" t="s">
         <v>65</v>
@@ -1736,7 +2933,7 @@
       </c>
       <c r="E46" s="20"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="32"/>
       <c r="B47" s="26" t="s">
         <v>66</v>
@@ -1747,7 +2944,7 @@
       </c>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="32"/>
       <c r="B48" s="26" t="s">
         <v>67</v>
@@ -1758,7 +2955,7 @@
       </c>
       <c r="E48" s="20"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="32"/>
       <c r="B49" s="26" t="s">
         <v>68</v>
@@ -1769,7 +2966,7 @@
       </c>
       <c r="E49" s="20"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="32"/>
       <c r="B50" s="26" t="s">
         <v>69</v>
@@ -1780,7 +2977,7 @@
       </c>
       <c r="E50" s="20"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="32"/>
       <c r="B51" s="26" t="s">
         <v>70</v>
@@ -1791,7 +2988,7 @@
       </c>
       <c r="E51" s="20"/>
     </row>
-    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A52" s="33"/>
       <c r="B52" s="27" t="s">
         <v>71</v>
@@ -1821,17 +3018,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1839,7 +3036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="30">
         <v>7.0159375299999993E-2</v>
       </c>
@@ -1847,7 +3044,7 @@
         <v>230.2535546</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="30">
         <v>50.662052770000003</v>
       </c>
@@ -1855,7 +3052,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="30">
         <v>157.92182149999999</v>
       </c>
@@ -1863,7 +3060,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="30">
         <v>265.18159020000002</v>
       </c>
@@ -1871,7 +3068,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="30">
         <v>372.44135899999998</v>
       </c>
@@ -1879,7 +3076,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="30">
         <v>479.70112769999997</v>
       </c>
@@ -1890,7 +3087,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="30">
         <v>586.96089640000002</v>
       </c>
@@ -1898,7 +3095,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="30">
         <v>694.22066510000002</v>
       </c>
@@ -1906,7 +3103,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="30">
         <v>801.78514910000001</v>
       </c>
@@ -1914,7 +3111,7 @@
         <v>230.3330272</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="30">
         <v>908.74020259999998</v>
       </c>
@@ -1922,7 +3119,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="30">
         <v>1015.999971</v>
       </c>
@@ -1930,7 +3127,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A13" s="30">
         <v>1123.25974</v>
       </c>
@@ -1938,7 +3135,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="30">
         <v>1230.519509</v>
       </c>
@@ -1946,7 +3143,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="30">
         <v>1331.075542</v>
       </c>
@@ -1954,7 +3151,7 @@
         <v>230.21973080000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="30">
         <v>1438.335311</v>
       </c>
@@ -1962,7 +3159,7 @@
         <v>220.41915</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="30">
         <v>1545.5950789999999</v>
       </c>
@@ -1970,7 +3167,7 @@
         <v>205.12270710000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="30">
         <v>1652.8548479999999</v>
       </c>
@@ -1978,7 +3175,7 @@
         <v>191.8115478</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19" s="30">
         <v>1760.114617</v>
       </c>
@@ -1986,7 +3183,7 @@
         <v>180.12272809999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A20" s="30">
         <v>1867.374386</v>
       </c>
@@ -1994,7 +3191,7 @@
         <v>169.7766924</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="30">
         <v>1974.6341540000001</v>
       </c>
@@ -2002,7 +3199,7 @@
         <v>160.5546253</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A22" s="30">
         <v>2081.8939230000001</v>
       </c>
@@ -2010,7 +3207,7 @@
         <v>152.28280520000001</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A23" s="30">
         <v>2189.1536919999999</v>
       </c>
@@ -2018,7 +3215,7 @@
         <v>144.8215572</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A24" s="30">
         <v>2296.4134610000001</v>
       </c>
@@ -2026,7 +3223,7 @@
         <v>138.05730199999999</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="30">
         <v>2403.3685139999998</v>
       </c>
@@ -2034,7 +3231,7 @@
         <v>131.913456</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A26" s="30">
         <v>2510.9329980000002</v>
       </c>
@@ -2042,7 +3239,7 @@
         <v>126.2624876</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A27" s="30">
         <v>2612.6063199999999</v>
       </c>
@@ -2050,7 +3247,7 @@
         <v>121.3488019</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A28" s="30">
         <v>2720.7599209999998</v>
       </c>
@@ -2058,7 +3255,7 @@
         <v>116.5250356</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="30">
         <v>2826.0085690000001</v>
       </c>
@@ -2066,7 +3263,7 @@
         <v>112.1853097</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30" s="30">
         <v>2933.268337</v>
       </c>
@@ -2074,7 +3271,7 @@
         <v>108.0830699</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A31" s="30">
         <v>3040.5281060000002</v>
       </c>
@@ -2082,7 +3279,7 @@
         <v>104.27025690000001</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="30">
         <v>3140.0879020000002</v>
       </c>
@@ -2090,7 +3287,7 @@
         <v>100.9642585</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A33" s="30">
         <v>3210.749726</v>
       </c>
@@ -2098,7 +3295,7 @@
         <v>98.742248290000006</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="30">
         <v>3309.794817</v>
       </c>
@@ -2106,7 +3303,7 @@
         <v>95.787401990000006</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="30">
         <v>3415.9372969999999</v>
       </c>
@@ -2114,7 +3311,7 @@
         <v>92.811026400000003</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A36" s="30">
         <v>3523.1970649999998</v>
       </c>
@@ -2122,7 +3319,7 @@
         <v>89.985499189999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37" s="30">
         <v>3630.4568340000001</v>
       </c>
@@ -2130,7 +3327,7 @@
         <v>87.326929129999996</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A38" s="30">
         <v>3737.7166029999998</v>
       </c>
@@ -2138,7 +3335,7 @@
         <v>84.820942919999993</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A39" s="30">
         <v>3844.9763720000001</v>
       </c>
@@ -2146,7 +3343,7 @@
         <v>82.454771100000002</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A40" s="30">
         <v>3945.5324049999999</v>
       </c>
@@ -2154,7 +3351,7 @@
         <v>80.353324749999999</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A41" s="30">
         <v>4053.7063189999999</v>
       </c>
@@ -2162,7 +3359,7 @@
         <v>78.209081190000006</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A42" s="30">
         <v>4160.0519420000001</v>
       </c>
@@ -2170,7 +3367,7 @@
         <v>76.209780809999998</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A43" s="30">
         <v>4267.3117110000003</v>
       </c>
@@ -2178,7 +3375,7 @@
         <v>74.294232089999994</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A44" s="30">
         <v>4374.5714799999996</v>
       </c>
@@ -2186,7 +3383,7 @@
         <v>72.472617740000004</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A45" s="30">
         <v>4480.9171029999998</v>
       </c>
@@ -2194,7 +3391,7 @@
         <v>70.752624819999994</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A46" s="30">
         <v>4589.0910169999997</v>
       </c>
@@ -2202,7 +3399,7 @@
         <v>69.084846099999993</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A47" s="30">
         <v>4694.3396650000004</v>
       </c>
@@ -2210,7 +3407,7 @@
         <v>67.535940999999994</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A48" s="30">
         <v>4801.4775479999998</v>
       </c>
@@ -2218,7 +3415,7 @@
         <v>66.028976180000001</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A49" s="30">
         <v>4907.5184550000004</v>
       </c>
@@ -2226,7 +3423,7 @@
         <v>64.602232180000001</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A50" s="30">
         <v>5014.7782239999997</v>
       </c>
@@ -2234,7 +3431,7 @@
         <v>63.22047207</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A51" s="30">
         <v>5122.0379929999999</v>
       </c>
@@ -2242,7 +3439,7 @@
         <v>61.896582389999999</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A52" s="30">
         <v>5227.957015</v>
       </c>
@@ -2250,7 +3447,7 @@
         <v>60.642550370000002</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A53" s="30">
         <v>5326.5019270000003</v>
       </c>
@@ -2258,7 +3455,7 @@
         <v>59.520610519999998</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A54" s="30">
         <v>5433.4569810000003</v>
       </c>
@@ -2269,8 +3466,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>